<commit_message>
Prepared pointspotdir for integration with program
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -723,11 +723,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="99608448"/>
-        <c:axId val="99609984"/>
+        <c:axId val="101320576"/>
+        <c:axId val="101322112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99608448"/>
+        <c:axId val="101320576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99609984"/>
+        <c:crossAx val="101322112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -744,7 +744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99609984"/>
+        <c:axId val="101322112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99608448"/>
+        <c:crossAx val="101320576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1108,7 +1108,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
@@ -1788,21 +1788,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012D17D2DA77674180682A0AA120B05E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87ee3a9c76d1b733a38dbfe83ae64a50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1851,10 +1836,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1868,16 +1875,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Textured tree Added lighting
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -723,11 +723,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101320576"/>
-        <c:axId val="101322112"/>
+        <c:axId val="100927360"/>
+        <c:axId val="100928896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101320576"/>
+        <c:axId val="100927360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101322112"/>
+        <c:crossAx val="100928896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -744,7 +744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101322112"/>
+        <c:axId val="100928896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101320576"/>
+        <c:crossAx val="100927360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1108,10 +1108,10 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1788,6 +1788,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012D17D2DA77674180682A0AA120B05E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87ee3a9c76d1b733a38dbfe83ae64a50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1836,32 +1851,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1875,9 +1868,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added light, view controls Added sunlight mode
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>Weighting</t>
   </si>
@@ -297,22 +297,19 @@
     <t>apply bumpmap shader to surface?</t>
   </si>
   <si>
-    <t>add input, sort final light values out</t>
-  </si>
-  <si>
     <t>instance grass</t>
   </si>
   <si>
-    <t>cache shader uniforms</t>
-  </si>
-  <si>
-    <t>add controls</t>
-  </si>
-  <si>
     <t>add tree view modes</t>
   </si>
   <si>
     <t>fire</t>
+  </si>
+  <si>
+    <t>lerp light colour? Background color?</t>
+  </si>
+  <si>
+    <t>speed</t>
   </si>
 </sst>
 </file>
@@ -686,7 +683,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.68112307692307705</c:v>
+                  <c:v>0.68596923076923078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,11 +735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103679872"/>
-        <c:axId val="103681408"/>
+        <c:axId val="100333440"/>
+        <c:axId val="100334976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103679872"/>
+        <c:axId val="100333440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103681408"/>
+        <c:crossAx val="100334976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103681408"/>
+        <c:axId val="100334976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103679872"/>
+        <c:crossAx val="100333440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1123,10 +1120,10 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1163,7 +1160,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.49384615384615388</v>
+        <v>0.50153846153846149</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1180,9 +1177,6 @@
       <c r="E4" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="G4" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
@@ -1198,9 +1192,6 @@
       <c r="E5" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
@@ -1214,10 +1205,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
         <v>48</v>
-      </c>
-      <c r="G6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1232,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1354,11 +1345,14 @@
       <c r="D16" s="20">
         <v>10</v>
       </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E16" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="18" t="s">
         <v>33</v>
@@ -1367,10 +1361,13 @@
         <v>1</v>
       </c>
       <c r="D17" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="18" t="s">
         <v>44</v>
@@ -1382,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
@@ -1395,11 +1392,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1411,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>8</v>
       </c>
@@ -1433,11 +1430,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>18</v>
       </c>
@@ -1449,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>20</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B27" s="18" t="s">
         <v>31</v>
       </c>
@@ -1471,7 +1468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="18" t="s">
         <v>21</v>
       </c>
@@ -1482,7 +1479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" s="18" t="s">
         <v>15</v>
       </c>
@@ -1493,11 +1490,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="s">
         <v>10</v>
       </c>
@@ -1507,10 +1504,10 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.49384615384615388</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.50153846153846149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="33" t="s">
         <v>9</v>
       </c>
@@ -1520,7 +1517,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.64569230769230779</v>
+        <v>0.65107692307692311</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1546,7 +1543,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.57483076923076926</v>
+        <v>0.58129230769230766</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1569,7 +1566,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.49384615384615388</v>
+        <v>0.50153846153846149</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1721,7 +1718,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.64569230769230779</v>
+        <v>0.65107692307692311</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1734,7 +1731,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.64569230769230779</v>
+        <v>0.65107692307692311</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1760,7 +1757,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.68112307692307705</v>
+        <v>0.68596923076923078</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added tree draw modes
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -683,7 +683,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.68596923076923078</c:v>
+                  <c:v>0.72716153846153853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,11 +735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="100333440"/>
-        <c:axId val="100334976"/>
+        <c:axId val="50988928"/>
+        <c:axId val="50990464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100333440"/>
+        <c:axId val="50988928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100334976"/>
+        <c:crossAx val="50990464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100334976"/>
+        <c:axId val="50990464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100333440"/>
+        <c:crossAx val="50988928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1120,10 +1120,10 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.50153846153846149</v>
+        <v>0.56692307692307697</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1331,7 +1331,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="20">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="20">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="F17" t="s">
         <v>51</v>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.50153846153846149</v>
+        <v>0.56692307692307697</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.65107692307692311</v>
+        <v>0.69684615384615389</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.58129230769230766</v>
+        <v>0.63621538461538463</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.50153846153846149</v>
+        <v>0.56692307692307697</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.65107692307692311</v>
+        <v>0.69684615384615389</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.65107692307692311</v>
+        <v>0.69684615384615389</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.68596923076923078</v>
+        <v>0.72716153846153853</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed wireframe in reflection
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -735,11 +735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50988928"/>
-        <c:axId val="50990464"/>
+        <c:axId val="102303616"/>
+        <c:axId val="102305152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50988928"/>
+        <c:axId val="102303616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50990464"/>
+        <c:crossAx val="102305152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50990464"/>
+        <c:axId val="102305152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50988928"/>
+        <c:crossAx val="102303616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1120,10 +1120,10 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1818,6 +1818,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012D17D2DA77674180682A0AA120B05E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87ee3a9c76d1b733a38dbfe83ae64a50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1866,32 +1881,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1905,9 +1898,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added snow, fixed pond draw order
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Weighting</t>
   </si>
@@ -683,7 +683,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.72716153846153853</c:v>
+                  <c:v>0.78531538461538453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,11 +735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102303616"/>
-        <c:axId val="102305152"/>
+        <c:axId val="100988800"/>
+        <c:axId val="100990336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102303616"/>
+        <c:axId val="100988800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102305152"/>
+        <c:crossAx val="100990336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102305152"/>
+        <c:axId val="100990336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102303616"/>
+        <c:crossAx val="100988800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1120,10 +1120,10 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.56692307692307697</v>
+        <v>0.65923076923076918</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1304,7 +1304,10 @@
         <v>6</v>
       </c>
       <c r="D13" s="20">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1504,7 +1507,7 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.56692307692307697</v>
+        <v>0.65923076923076918</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1517,7 +1520,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.69684615384615389</v>
+        <v>0.76146153846153841</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1543,7 +1546,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.63621538461538463</v>
+        <v>0.71375384615384607</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1566,7 +1569,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.56692307692307697</v>
+        <v>0.65923076923076918</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1718,7 +1721,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.69684615384615389</v>
+        <v>0.76146153846153841</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1731,7 +1734,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.69684615384615389</v>
+        <v>0.76146153846153841</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1757,7 +1760,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.72716153846153853</v>
+        <v>0.78531538461538453</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -1818,21 +1821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012D17D2DA77674180682A0AA120B05E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87ee3a9c76d1b733a38dbfe83ae64a50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1881,10 +1869,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1898,16 +1908,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Leaves now grow and fall off tree
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Weighting</t>
   </si>
@@ -683,7 +683,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.78531538461538453</c:v>
+                  <c:v>0.80470000000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,11 +735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="100988800"/>
-        <c:axId val="100990336"/>
+        <c:axId val="86046592"/>
+        <c:axId val="86048128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100988800"/>
+        <c:axId val="86046592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100990336"/>
+        <c:crossAx val="86048128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100990336"/>
+        <c:axId val="86048128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100988800"/>
+        <c:crossAx val="86046592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1123,7 +1123,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.65923076923076918</v>
+        <v>0.69000000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1280,7 +1280,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="20">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1507,7 +1510,7 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.65923076923076918</v>
+        <v>0.69000000000000006</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1520,7 +1523,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.76146153846153841</v>
+        <v>0.78300000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1546,7 +1549,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.71375384615384607</v>
+        <v>0.73959999999999992</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1569,7 +1572,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.65923076923076918</v>
+        <v>0.69000000000000006</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1721,7 +1724,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.76146153846153841</v>
+        <v>0.78300000000000003</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1734,7 +1737,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.76146153846153841</v>
+        <v>0.78300000000000003</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1760,7 +1763,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.78531538461538453</v>
+        <v>0.80470000000000008</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed light saturation in spotlight overlap Added snowdrift
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Weighting</t>
   </si>
@@ -300,16 +300,19 @@
     <t>instance grass</t>
   </si>
   <si>
-    <t>add tree view modes</t>
-  </si>
-  <si>
-    <t>fire</t>
-  </si>
-  <si>
     <t>lerp light colour? Background color?</t>
   </si>
   <si>
     <t>speed</t>
+  </si>
+  <si>
+    <t>flip lights for reflection</t>
+  </si>
+  <si>
+    <t>fire, lightning, seasons</t>
+  </si>
+  <si>
+    <t>flat shaded version of leaves?</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.80470000000000008</c:v>
+                  <c:v>0.86285384615384608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,11 +738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="86046592"/>
-        <c:axId val="86048128"/>
+        <c:axId val="101578624"/>
+        <c:axId val="101580160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86046592"/>
+        <c:axId val="101578624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86048128"/>
+        <c:crossAx val="101580160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86048128"/>
+        <c:axId val="101580160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86046592"/>
+        <c:crossAx val="101578624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1123,7 +1126,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1160,7 +1163,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.69000000000000006</v>
+        <v>0.78230769230769226</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1177,6 +1180,9 @@
       <c r="E4" s="44" t="s">
         <v>45</v>
       </c>
+      <c r="G4" s="45" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
@@ -1207,9 +1213,6 @@
       <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
@@ -1220,10 +1223,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="20">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1339,6 +1342,9 @@
       <c r="D15" s="20">
         <v>8</v>
       </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
@@ -1355,6 +1361,9 @@
         <v>45</v>
       </c>
       <c r="F16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="45" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1370,7 +1379,7 @@
         <v>7.5</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1510,7 +1519,7 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.69000000000000006</v>
+        <v>0.78230769230769226</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1523,7 +1532,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.78300000000000003</v>
+        <v>0.84761538461538455</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1549,7 +1558,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.73959999999999992</v>
+        <v>0.81713846153846137</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1572,7 +1581,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.69000000000000006</v>
+        <v>0.78230769230769226</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1724,7 +1733,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.78300000000000003</v>
+        <v>0.84761538461538455</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1737,7 +1746,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.78300000000000003</v>
+        <v>0.84761538461538455</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1763,7 +1772,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.80470000000000008</v>
+        <v>0.86285384615384608</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Snow can now transition in and out Added Season transitions
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Weighting</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>lerp light colour? Background color?</t>
-  </si>
-  <si>
-    <t>speed</t>
   </si>
   <si>
     <t>flip lights for reflection</t>
@@ -686,7 +683,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.86285384615384608</c:v>
+                  <c:v>0.86527692307692317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,11 +735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101578624"/>
-        <c:axId val="101580160"/>
+        <c:axId val="102565760"/>
+        <c:axId val="102567296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101578624"/>
+        <c:axId val="102565760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101580160"/>
+        <c:crossAx val="102567296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101580160"/>
+        <c:axId val="102567296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101578624"/>
+        <c:crossAx val="102565760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1126,7 +1123,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1163,7 +1160,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.78230769230769226</v>
+        <v>0.78615384615384609</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1181,7 +1178,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1343,7 +1340,7 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1364,10 +1361,10 @@
         <v>48</v>
       </c>
       <c r="G16" s="45" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="18" t="s">
         <v>33</v>
@@ -1376,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="D17" s="20">
-        <v>7.5</v>
-      </c>
-      <c r="F17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="18" t="s">
         <v>44</v>
@@ -1394,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
@@ -1407,11 +1404,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>9</v>
       </c>
@@ -1423,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
         <v>7</v>
       </c>
@@ -1434,7 +1431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>8</v>
       </c>
@@ -1445,11 +1442,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>18</v>
       </c>
@@ -1461,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>20</v>
       </c>
@@ -1472,7 +1469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B27" s="18" t="s">
         <v>31</v>
       </c>
@@ -1483,7 +1480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="18" t="s">
         <v>21</v>
       </c>
@@ -1494,7 +1491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="18" t="s">
         <v>15</v>
       </c>
@@ -1505,11 +1502,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="s">
         <v>10</v>
       </c>
@@ -1519,10 +1516,10 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.78230769230769226</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.78615384615384609</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="33" t="s">
         <v>9</v>
       </c>
@@ -1532,7 +1529,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.84761538461538455</v>
+        <v>0.85030769230769232</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1558,7 +1555,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.81713846153846137</v>
+        <v>0.82036923076923074</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1581,7 +1578,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.78230769230769226</v>
+        <v>0.78615384615384609</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1733,7 +1730,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.84761538461538455</v>
+        <v>0.85030769230769232</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1746,7 +1743,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.84761538461538455</v>
+        <v>0.85030769230769232</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1772,7 +1769,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.86285384615384608</v>
+        <v>0.86527692307692317</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -1833,6 +1830,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012D17D2DA77674180682A0AA120B05E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87ee3a9c76d1b733a38dbfe83ae64a50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1881,32 +1893,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1920,9 +1910,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Smoke Particle system is now a re-useable particle emitter system Added fire emitter
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Weighting</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>flat shaded version of leaves?</t>
+  </si>
+  <si>
+    <t>better blend mode?</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.86527692307692317</c:v>
+                  <c:v>0.90404615384615383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,11 +738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102565760"/>
-        <c:axId val="102567296"/>
+        <c:axId val="115083136"/>
+        <c:axId val="115084672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102565760"/>
+        <c:axId val="115083136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102567296"/>
+        <c:crossAx val="115084672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102567296"/>
+        <c:axId val="115084672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102565760"/>
+        <c:crossAx val="115083136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1123,7 +1126,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1160,7 +1163,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.78615384615384609</v>
+        <v>0.84769230769230774</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1295,7 +1298,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="20">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -1516,7 +1525,7 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.78615384615384609</v>
+        <v>0.84769230769230774</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1529,7 +1538,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.85030769230769232</v>
+        <v>0.89338461538461544</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1555,7 +1564,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.82036923076923074</v>
+        <v>0.87206153846153844</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1578,7 +1587,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.78615384615384609</v>
+        <v>0.84769230769230774</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1730,7 +1739,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.85030769230769232</v>
+        <v>0.89338461538461544</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1743,7 +1752,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.85030769230769232</v>
+        <v>0.89338461538461544</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1769,7 +1778,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.86527692307692317</v>
+        <v>0.90404615384615383</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added Tree Config File
</commit_message>
<xml_diff>
--- a/08960-1 Mark Scheme 11-12.xlsx
+++ b/08960-1 Mark Scheme 11-12.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Weighting</t>
   </si>
@@ -686,7 +686,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.90404615384615383</c:v>
+                  <c:v>0.93312307692307694</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,11 +738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="94050176"/>
-        <c:axId val="94051712"/>
+        <c:axId val="173348736"/>
+        <c:axId val="173350272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94050176"/>
+        <c:axId val="173348736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94051712"/>
+        <c:crossAx val="173350272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94051712"/>
+        <c:axId val="173350272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94050176"/>
+        <c:crossAx val="173348736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1126,7 +1126,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="D3" s="4">
         <f>SUMPRODUCT($C4:$C19,D4:D19)/SUM($C4:$C19)/10</f>
-        <v>0.84769230769230774</v>
+        <v>0.89384615384615385</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1271,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E10" s="44" t="s">
         <v>45</v>
@@ -1400,7 +1400,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="20">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1528,7 +1531,7 @@
       </c>
       <c r="D31" s="42">
         <f>D3</f>
-        <v>0.84769230769230774</v>
+        <v>0.89384615384615385</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1541,7 +1544,7 @@
       </c>
       <c r="D32" s="43">
         <f>D21*(D3*$C3 + (1-$C3 ))</f>
-        <v>0.89338461538461544</v>
+        <v>0.9256923076923077</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1567,7 +1570,7 @@
       </c>
       <c r="D34" s="29">
         <f>SUMPRODUCT($C31:$C33,D31:D33)</f>
-        <v>0.87206153846153844</v>
+        <v>0.91083076923076922</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1590,7 +1593,7 @@
       </c>
       <c r="D37" s="4">
         <f>D3</f>
-        <v>0.84769230769230774</v>
+        <v>0.89384615384615385</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1742,7 +1745,7 @@
       </c>
       <c r="D53" s="36">
         <f>D39*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.89338461538461544</v>
+        <v>0.9256923076923077</v>
       </c>
     </row>
     <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1755,7 +1758,7 @@
       </c>
       <c r="D54" s="39">
         <f>D46*(D37*$C37 + (1-$C37 ))</f>
-        <v>0.89338461538461544</v>
+        <v>0.9256923076923077</v>
       </c>
     </row>
     <row r="55" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.2">
@@ -1781,7 +1784,7 @@
       </c>
       <c r="D56" s="29">
         <f>SUMPRODUCT($C53:$C55,D53:D55)</f>
-        <v>0.90404615384615383</v>
+        <v>0.93312307692307694</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -1842,6 +1845,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012D17D2DA77674180682A0AA120B05E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="87ee3a9c76d1b733a38dbfe83ae64a50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1890,32 +1908,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1929,9 +1925,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3251BF-7063-456F-AB34-DBC92B3DAB4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF29B442-1189-4473-8918-DD97B228EF99}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>